<commit_message>
update fields missing n: to make process-able in R
</commit_message>
<xml_diff>
--- a/data/Field_data/HZ19_FACS_complete.xlsx
+++ b/data/Field_data/HZ19_FACS_complete.xlsx
@@ -3850,7 +3850,7 @@
     <t xml:space="preserve">57.0 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_763_001.fcs</t>
+    <t xml:space="preserve">1: spleen_763_001.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">94.3 %</t>
@@ -3859,7 +3859,7 @@
     <t xml:space="preserve">7.45 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_764_002.fcs</t>
+    <t xml:space="preserve">1: spleen_764_002.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">7.90 %</t>
@@ -3874,7 +3874,7 @@
     <t xml:space="preserve">31.3 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_765_003.fcs</t>
+    <t xml:space="preserve">1: spleen_765_003.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">5.05 %</t>
@@ -3895,7 +3895,7 @@
     <t xml:space="preserve">2.39 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_766_004.fcs</t>
+    <t xml:space="preserve">1: spleen_766_004.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">45.2 %</t>
@@ -3919,7 +3919,7 @@
     <t xml:space="preserve">2.44 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_767_005.fcs</t>
+    <t xml:space="preserve">1: spleen_767_005.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">26.3 %</t>
@@ -3928,7 +3928,7 @@
     <t xml:space="preserve">1.21 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_768_006.fcs</t>
+    <t xml:space="preserve">1: spleen_768_006.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">90.1 %</t>
@@ -3946,7 +3946,7 @@
     <t xml:space="preserve">1.13 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_769_007.fcs</t>
+    <t xml:space="preserve">1: spleen_769_007.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">6.13 %</t>
@@ -3961,7 +3961,7 @@
     <t xml:space="preserve">4.75 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_770_008.fcs</t>
+    <t xml:space="preserve">1: spleen_770_008.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">29.6 %</t>
@@ -3979,7 +3979,7 @@
     <t xml:space="preserve">9.99 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_771_009.fcs</t>
+    <t xml:space="preserve">1: spleen_771_009.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">8.22 %</t>
@@ -3988,7 +3988,7 @@
     <t xml:space="preserve">17.8 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_772_010.fcs</t>
+    <t xml:space="preserve">1: spleen_772_010.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">5.85 %</t>
@@ -3997,7 +3997,7 @@
     <t xml:space="preserve">45.7 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_773_011.fcs</t>
+    <t xml:space="preserve">1: spleen_773_011.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">2.86 %</t>
@@ -4006,7 +4006,7 @@
     <t xml:space="preserve">8.61 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_774_012.fcs</t>
+    <t xml:space="preserve">1: spleen_774_012.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">4.29 %</t>
@@ -4030,7 +4030,7 @@
     <t xml:space="preserve">3.35 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_775_013.fcs</t>
+    <t xml:space="preserve">1: spleen_775_013.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">3.25 %</t>
@@ -4045,19 +4045,19 @@
     <t xml:space="preserve">38.8 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_776_014.fcs</t>
+    <t xml:space="preserve">1: spleen_776_014.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">47.1 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_777_015.fcs</t>
+    <t xml:space="preserve">1: spleen_777_015.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">8.13 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_778_016.fcs</t>
+    <t xml:space="preserve">1: spleen_778_016.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">49.9 %</t>
@@ -4069,7 +4069,7 @@
     <t xml:space="preserve">8.00 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_779_017.fcs</t>
+    <t xml:space="preserve">1: spleen_779_017.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">8.75 %</t>
@@ -4078,7 +4078,7 @@
     <t xml:space="preserve">7.73 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_780_018.fcs</t>
+    <t xml:space="preserve">1: spleen_780_018.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">3.92 %</t>
@@ -4093,7 +4093,7 @@
     <t xml:space="preserve">28.9 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_781_019.fcs</t>
+    <t xml:space="preserve">1: spleen_781_019.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">5.10 %</t>
@@ -4111,7 +4111,7 @@
     <t xml:space="preserve">3.06 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_782_020.fcs</t>
+    <t xml:space="preserve">1: spleen_782_020.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">52.8 %</t>
@@ -4123,7 +4123,7 @@
     <t xml:space="preserve">47.0 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_783_021.fcs</t>
+    <t xml:space="preserve">1: spleen_783_021.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">8.50 %</t>
@@ -4135,13 +4135,13 @@
     <t xml:space="preserve">2.25 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_784_022.fcs</t>
+    <t xml:space="preserve">1: spleen_784_022.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">91.4 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_785_023.fcs</t>
+    <t xml:space="preserve">1: spleen_785_023.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">7.99 %</t>
@@ -4156,7 +4156,7 @@
     <t xml:space="preserve">0.20 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_786_024.fcs</t>
+    <t xml:space="preserve">1: spleen_786_024.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">83.7 %</t>
@@ -4165,7 +4165,7 @@
     <t xml:space="preserve">6.63 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_787_025.fcs</t>
+    <t xml:space="preserve">1: spleen_787_025.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">2.95 %</t>
@@ -4174,7 +4174,7 @@
     <t xml:space="preserve">90.8 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_788_026.fcs</t>
+    <t xml:space="preserve">1: spleen_788_026.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">6.88 %</t>
@@ -4186,7 +4186,7 @@
     <t xml:space="preserve">93.1 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_789_027.fcs</t>
+    <t xml:space="preserve">1: spleen_789_027.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">34.3 %</t>
@@ -4201,13 +4201,13 @@
     <t xml:space="preserve">15.5 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_790_028.fcs</t>
+    <t xml:space="preserve">1: spleen_790_028.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">8.84 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_791_029.fcs</t>
+    <t xml:space="preserve">1: spleen_791_029.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">7.86 %</t>
@@ -4216,7 +4216,7 @@
     <t xml:space="preserve">0.31 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_792_030.fcs</t>
+    <t xml:space="preserve">1: spleen_792_030.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">49.1 %</t>
@@ -4225,7 +4225,7 @@
     <t xml:space="preserve">8.09 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_793_031.fcs</t>
+    <t xml:space="preserve">1: spleen_793_031.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">1.83 %</t>
@@ -4234,7 +4234,7 @@
     <t xml:space="preserve">1.26 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_794_032.fcs</t>
+    <t xml:space="preserve">1: spleen_794_032.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">67.4 %</t>
@@ -4243,7 +4243,7 @@
     <t xml:space="preserve">8.27 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_795_033.fcs</t>
+    <t xml:space="preserve">1: spleen_795_033.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">1.56 %</t>
@@ -4258,7 +4258,7 @@
     <t xml:space="preserve">9.89 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_796_034.fcs</t>
+    <t xml:space="preserve">1: spleen_796_034.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">3.93 %</t>
@@ -4273,7 +4273,7 @@
     <t xml:space="preserve">2.75 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_797_035.fcs</t>
+    <t xml:space="preserve">1: spleen_797_035.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">1.73 %</t>
@@ -4285,13 +4285,13 @@
     <t xml:space="preserve">60.1 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_798_036.fcs</t>
+    <t xml:space="preserve">1: spleen_798_036.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">2.30 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_799_037.fcs</t>
+    <t xml:space="preserve">1: spleen_799_037.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">86.5 %</t>
@@ -4300,7 +4300,7 @@
     <t xml:space="preserve">7.44 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_800_038.fcs</t>
+    <t xml:space="preserve">1: spleen_800_038.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">41.6 %</t>
@@ -4318,7 +4318,7 @@
     <t xml:space="preserve">48.2 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_801_039.fcs</t>
+    <t xml:space="preserve">1: spleen_801_039.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">1.40 %</t>
@@ -4327,7 +4327,7 @@
     <t xml:space="preserve">0.097 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_802_040.fcs</t>
+    <t xml:space="preserve">1: spleen_802_040.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">9.93 %</t>
@@ -4342,13 +4342,13 @@
     <t xml:space="preserve">0.017 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_803_041.fcs</t>
+    <t xml:space="preserve">1: spleen_803_041.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">80.2 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_804_042.fcs</t>
+    <t xml:space="preserve">1: spleen_804_042.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">29.7 %</t>
@@ -4363,7 +4363,7 @@
     <t xml:space="preserve">2.11 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_805_043.fcs</t>
+    <t xml:space="preserve">1: spleen_805_043.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">37.3 %</t>
@@ -4375,7 +4375,7 @@
     <t xml:space="preserve">4.87 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_806_044.fcs</t>
+    <t xml:space="preserve">1: spleen_806_044.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">43.8 %</t>
@@ -4390,7 +4390,7 @@
     <t xml:space="preserve">3.83 %</t>
   </si>
   <si>
-    <t xml:space="preserve">spleen_807_045.fcs</t>
+    <t xml:space="preserve">1: spleen_807_045.fcs</t>
   </si>
   <si>
     <t xml:space="preserve">80.5 %</t>
@@ -4596,14 +4596,14 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q30" activeCellId="0" sqref="Q30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C154" activeCellId="0" sqref="C154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.5"/>
@@ -4611,14 +4611,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="42.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="37.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="46.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="46.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="31.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="44.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="17" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>

</xml_diff>